<commit_message>
Modified Aerosol, Atmos, Seaice for ES2L, dealing with the review comments.
</commit_message>
<xml_diff>
--- a/cmip6/models/miroc-es2l/cmip6_miroc_miroc-es2l_atmos.xlsx
+++ b/cmip6/models/miroc-es2l/cmip6_miroc_miroc-es2l_atmos.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23517"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="233" documentId="11_5D484C3A59773848156225B544A42272D33F279A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{76FA519B-6224-4E3E-A7C5-CCB2B23221F8}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4d566ba9b8f1570b/仕事/ES-DOC/SharedForWriters/models/miroc-es2l/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="272" documentId="11_5D484C3A59773848156225B544A42272D33F279A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2F0D3396-05E8-406F-A68D-5093415F074D}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" firstSheet="9" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14620" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -21,7 +26,7 @@
     <sheet name="9. Gravity Waves" sheetId="11" r:id="rId11"/>
     <sheet name="10. Natural Forcing" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2575" uniqueCount="1238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2604" uniqueCount="1243">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -700,9 +705,6 @@
     <t>Scheme Method</t>
   </si>
   <si>
-    <t>Horizontal discretisation method</t>
-  </si>
-  <si>
     <t>cmip6.atmos.grid.discretisation.horizontal.scheme_method</t>
   </si>
   <si>
@@ -728,6 +730,9 @@
   </si>
   <si>
     <t>cmip6.atmos.grid.discretisation.horizontal.scheme_order</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
   <si>
     <t>second</t>
@@ -3814,17 +3819,37 @@
   </si>
   <si>
     <t>stratospheric aerosols optical thickness</t>
+  </si>
+  <si>
+    <t>Horizontal discretisation method</t>
+    <phoneticPr fontId="16"/>
+  </si>
+  <si>
+    <t>Spectral</t>
+    <phoneticPr fontId="16"/>
+  </si>
+  <si>
+    <t>T42L40</t>
+    <phoneticPr fontId="16"/>
+  </si>
+  <si>
+    <t>Not needed</t>
+    <phoneticPr fontId="16"/>
+  </si>
+  <si>
+    <t>Not considering cloud inhomogeneity</t>
+    <phoneticPr fontId="16"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3924,6 +3949,13 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
@@ -4039,7 +4071,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4363,19 +4395,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.7265625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.7265625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="32.5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="20">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -4383,7 +4415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="20">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -4391,7 +4423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="20">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -4399,7 +4431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="20">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -4407,7 +4439,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="20">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -4415,52 +4447,52 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" ht="20">
       <c r="B10" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="20">
       <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="20">
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="20">
       <c r="B13" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="20">
       <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" ht="20">
       <c r="B15" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="20">
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="20">
       <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" ht="17.5">
       <c r="A19" s="5" t="s">
         <v>20</v>
       </c>
@@ -4468,7 +4500,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" ht="17.5">
       <c r="A20" s="5" t="s">
         <v>22</v>
       </c>
@@ -4476,7 +4508,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" ht="17.5">
       <c r="A21" s="5" t="s">
         <v>24</v>
       </c>
@@ -4484,7 +4516,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" ht="17.5">
       <c r="A22" s="5" t="s">
         <v>26</v>
       </c>
@@ -4492,19 +4524,20 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" ht="20">
       <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B24" s="4"/>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" ht="20">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B25" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <hyperlinks>
     <hyperlink ref="B19" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B20" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
@@ -4521,12 +4554,12 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -4590,7 +4623,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="177.95" customHeight="1">
+    <row r="11" spans="1:3" ht="178" customHeight="1">
       <c r="B11" s="11" t="s">
         <v>983</v>
       </c>
@@ -5009,6 +5042,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{74914CC9-FC1F-4E36-8BD5-CC4736030174}">
       <formula1>AA20:AD20</formula1>
@@ -5035,16 +5069,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:AF76"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="24" customHeight="1">
@@ -5108,7 +5142,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="177.95" customHeight="1">
+    <row r="11" spans="1:29" ht="178" customHeight="1">
       <c r="B11" s="11" t="s">
         <v>1072</v>
       </c>
@@ -5489,7 +5523,12 @@
       </c>
     </row>
     <row r="63" spans="1:32" ht="24" customHeight="1">
-      <c r="B63" s="11"/>
+      <c r="B63" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D63" s="6" t="s">
+        <v>217</v>
+      </c>
       <c r="AA63" s="6" t="s">
         <v>1145</v>
       </c>
@@ -5556,7 +5595,12 @@
       </c>
     </row>
     <row r="72" spans="1:32" ht="24" customHeight="1">
-      <c r="B72" s="11"/>
+      <c r="B72" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>217</v>
+      </c>
       <c r="AA72" s="6" t="s">
         <v>1124</v>
       </c>
@@ -5587,7 +5631,12 @@
       </c>
     </row>
     <row r="76" spans="1:32" ht="24" customHeight="1">
-      <c r="B76" s="11"/>
+      <c r="B76" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>217</v>
+      </c>
       <c r="AA76" s="6" t="s">
         <v>1132</v>
       </c>
@@ -5608,6 +5657,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15 B72 B19 B42" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>AA15:AC15</formula1>
@@ -5632,12 +5682,12 @@
   <sheetViews>
     <sheetView topLeftCell="A66" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -5699,7 +5749,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="177.95" customHeight="1">
+    <row r="11" spans="1:3" ht="178" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -6037,7 +6087,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:29" ht="177.95" customHeight="1">
+    <row r="73" spans="1:29" ht="178" customHeight="1">
       <c r="B73" s="11" t="s">
         <v>1230</v>
       </c>
@@ -6076,6 +6126,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <dataValidations count="6">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20" xr:uid="{81DE60D9-C1B1-4DAE-901B-DD88028420B2}">
       <formula1>AA20:AD20</formula1>
@@ -6098,6 +6149,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6109,14 +6161,14 @@
       <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="80.7265625" customWidth="1"/>
+    <col min="2" max="2" width="40.7265625" customWidth="1"/>
+    <col min="3" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30">
       <c r="A1" s="7" t="s">
         <v>30</v>
       </c>
@@ -6127,7 +6179,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="18">
       <c r="A5" s="9" t="s">
         <v>32</v>
       </c>
@@ -6151,7 +6203,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="18">
+    <row r="9" spans="1:2" ht="17.5">
       <c r="A9" s="11" t="s">
         <v>37</v>
       </c>
@@ -6159,7 +6211,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="18">
+    <row r="10" spans="1:2" ht="17.5">
       <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
@@ -6167,7 +6219,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="18">
+    <row r="11" spans="1:2" ht="17.5">
       <c r="A11" s="11" t="s">
         <v>40</v>
       </c>
@@ -6175,7 +6227,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="18">
+    <row r="12" spans="1:2" ht="17.5">
       <c r="A12" s="11" t="s">
         <v>41</v>
       </c>
@@ -6183,7 +6235,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="18">
+    <row r="13" spans="1:2" ht="17.5">
       <c r="A13" s="11" t="s">
         <v>42</v>
       </c>
@@ -6191,7 +6243,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="18">
+    <row r="14" spans="1:2" ht="17.5">
       <c r="A14" s="11" t="s">
         <v>43</v>
       </c>
@@ -6199,7 +6251,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="18">
+    <row r="15" spans="1:2" ht="17.5">
       <c r="A15" s="11" t="s">
         <v>44</v>
       </c>
@@ -6207,7 +6259,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="18">
+    <row r="16" spans="1:2" ht="17.5">
       <c r="A16" s="11" t="s">
         <v>45</v>
       </c>
@@ -6215,7 +6267,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="18">
+    <row r="17" spans="1:2" ht="17.5">
       <c r="A17" s="11" t="s">
         <v>46</v>
       </c>
@@ -6223,7 +6275,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="18">
+    <row r="18" spans="1:2" ht="17.5">
       <c r="A18" s="11" t="s">
         <v>47</v>
       </c>
@@ -6231,7 +6283,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="18">
+    <row r="19" spans="1:2" ht="17.5">
       <c r="A19" s="11" t="s">
         <v>48</v>
       </c>
@@ -6239,7 +6291,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="18">
+    <row r="20" spans="1:2" ht="17.5">
       <c r="A20" s="11" t="s">
         <v>49</v>
       </c>
@@ -6247,7 +6299,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="18">
+    <row r="21" spans="1:2" ht="17.5">
       <c r="A21" s="11" t="s">
         <v>50</v>
       </c>
@@ -6255,7 +6307,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="18">
+    <row r="22" spans="1:2" ht="17.5">
       <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
@@ -6263,7 +6315,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18">
+    <row r="23" spans="1:2" ht="17.5">
       <c r="A23" s="11" t="s">
         <v>52</v>
       </c>
@@ -6271,7 +6323,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18">
+    <row r="24" spans="1:2" ht="17.5">
       <c r="A24" s="11" t="s">
         <v>53</v>
       </c>
@@ -6279,7 +6331,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18">
+    <row r="25" spans="1:2" ht="17.5">
       <c r="A25" s="11" t="s">
         <v>54</v>
       </c>
@@ -6287,7 +6339,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="18">
+    <row r="26" spans="1:2" ht="17.5">
       <c r="A26" s="11" t="s">
         <v>55</v>
       </c>
@@ -6295,7 +6347,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="18">
+    <row r="27" spans="1:2" ht="17.5">
       <c r="A27" s="11" t="s">
         <v>57</v>
       </c>
@@ -6319,7 +6371,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75">
+    <row r="33" spans="1:2">
       <c r="A33" s="10" t="s">
         <v>35</v>
       </c>
@@ -6327,11 +6379,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="18">
+    <row r="34" spans="1:2" ht="17.5">
       <c r="A34" s="11"/>
       <c r="B34" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9:B27" xr:uid="{4B6CE098-85D1-4FDE-93C0-440243BE92B5}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
@@ -6352,16 +6405,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AG106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -6454,7 +6507,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="177.95" customHeight="1">
+    <row r="16" spans="1:3" ht="178" customHeight="1">
       <c r="B16" s="11" t="s">
         <v>82</v>
       </c>
@@ -6990,6 +7043,7 @@
       <c r="B106" s="11"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20 B73" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>AA20:AC20</formula1>
@@ -7015,16 +7069,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AF44"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -7060,7 +7114,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
+      <c r="B6" s="11" t="s">
+        <v>1240</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="24" customHeight="1">
       <c r="A8" s="9" t="s">
@@ -7086,7 +7142,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="177.95" customHeight="1">
+    <row r="11" spans="1:3" ht="178" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="14" spans="1:3" ht="24" customHeight="1">
@@ -7148,33 +7204,33 @@
         <v>85</v>
       </c>
       <c r="B22" s="10" t="s">
+        <v>1238</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>208</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="23" spans="1:30" ht="24" customHeight="1">
       <c r="B23" s="11"/>
       <c r="AA23" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="AB23" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="AB23" s="6" t="s">
+      <c r="AC23" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="AC23" s="6" t="s">
+      <c r="AD23" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="AD23" s="6" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:30" ht="24" customHeight="1">
       <c r="A25" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>214</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:30" ht="24" customHeight="1">
@@ -7182,14 +7238,19 @@
         <v>85</v>
       </c>
       <c r="B26" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="C26" s="10" t="s">
-        <v>217</v>
-      </c>
     </row>
     <row r="27" spans="1:30" ht="24" customHeight="1">
-      <c r="B27" s="11"/>
+      <c r="B27" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>1239</v>
+      </c>
       <c r="AA27" s="6" t="s">
         <v>218</v>
       </c>
@@ -7223,7 +7284,12 @@
       </c>
     </row>
     <row r="31" spans="1:30" ht="24" customHeight="1">
-      <c r="B31" s="11"/>
+      <c r="B31" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>1241</v>
+      </c>
       <c r="AA31" s="6" t="s">
         <v>225</v>
       </c>
@@ -7337,6 +7403,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <dataValidations count="4">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19" xr:uid="{C011DE76-C2A4-4D32-ADA6-1D6CFC478AC4}">
       <formula1>AA19:AC19</formula1>
@@ -7359,16 +7426,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AM109"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="A96" sqref="A96:XFD96"/>
+    <sheetView topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="A110" sqref="A110"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:36" ht="24" customHeight="1">
@@ -7430,7 +7497,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:36" ht="177.95" customHeight="1">
+    <row r="11" spans="1:36" ht="178" customHeight="1">
       <c r="B11" s="11"/>
     </row>
     <row r="13" spans="1:36" ht="24" customHeight="1">
@@ -7888,7 +7955,9 @@
       </c>
     </row>
     <row r="37" spans="1:29" ht="24" customHeight="1">
-      <c r="B37" s="11"/>
+      <c r="B37" s="11" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="39" spans="1:29" ht="24" customHeight="1">
       <c r="A39" s="9" t="s">
@@ -7910,7 +7979,9 @@
       </c>
     </row>
     <row r="41" spans="1:29" ht="24" customHeight="1">
-      <c r="B41" s="11"/>
+      <c r="B41" s="11" t="s">
+        <v>217</v>
+      </c>
     </row>
     <row r="44" spans="1:29" ht="24" customHeight="1">
       <c r="A44" s="12" t="s">
@@ -8341,7 +8412,12 @@
       </c>
     </row>
     <row r="100" spans="1:33" ht="24" customHeight="1">
-      <c r="B100" s="11"/>
+      <c r="B100" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>217</v>
+      </c>
       <c r="AA100" s="6" t="s">
         <v>392</v>
       </c>
@@ -8383,7 +8459,12 @@
       </c>
     </row>
     <row r="105" spans="1:33" ht="24" customHeight="1">
-      <c r="B105" s="11"/>
+      <c r="B105" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>217</v>
+      </c>
       <c r="AA105" s="6" t="s">
         <v>399</v>
       </c>
@@ -8426,7 +8507,12 @@
       </c>
     </row>
     <row r="109" spans="1:33" ht="24" customHeight="1">
-      <c r="B109" s="11"/>
+      <c r="B109" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>217</v>
+      </c>
       <c r="AA109" s="6" t="s">
         <v>368</v>
       </c>
@@ -8435,6 +8521,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <dataValidations count="8">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15" xr:uid="{247B5E13-C36D-44D7-B617-777B8953AD01}">
       <formula1>AA15:AJ15</formula1>
@@ -8469,16 +8556,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AX243"/>
   <sheetViews>
-    <sheetView topLeftCell="A219" workbookViewId="0">
-      <selection activeCell="A237" sqref="A237:XFD237"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="E111" sqref="E111"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" ht="24" customHeight="1">
@@ -8542,7 +8629,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:40" ht="177.95" customHeight="1">
+    <row r="11" spans="1:40" ht="178" customHeight="1">
       <c r="B11" s="15" t="s">
         <v>417</v>
       </c>
@@ -9847,7 +9934,12 @@
       </c>
     </row>
     <row r="111" spans="1:31" ht="24" customHeight="1">
-      <c r="B111" s="11"/>
+      <c r="B111" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>1242</v>
+      </c>
       <c r="AA111" s="6" t="s">
         <v>599</v>
       </c>
@@ -11802,7 +11894,12 @@
       </c>
     </row>
     <row r="228" spans="1:33" ht="24" customHeight="1">
-      <c r="B228" s="11"/>
+      <c r="B228" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D228" s="6" t="s">
+        <v>1242</v>
+      </c>
       <c r="AA228" s="6" t="s">
         <v>599</v>
       </c>
@@ -11953,6 +12050,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <dataValidations count="16">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16:B22" xr:uid="{065C6A09-8BF6-42DF-9650-3CCEC5967A35}">
       <formula1>AA16:AN16</formula1>
@@ -12011,16 +12109,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AK94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="G83" sqref="G83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -12082,7 +12180,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="177.95" customHeight="1">
+    <row r="11" spans="1:3" ht="178" customHeight="1">
       <c r="B11" s="11" t="s">
         <v>704</v>
       </c>
@@ -12764,7 +12862,12 @@
       </c>
     </row>
     <row r="80" spans="1:30" ht="24" customHeight="1">
-      <c r="B80" s="11"/>
+      <c r="B80" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>217</v>
+      </c>
       <c r="AA80" s="6" t="s">
         <v>747</v>
       </c>
@@ -12795,7 +12898,12 @@
       </c>
     </row>
     <row r="84" spans="1:32" ht="24" customHeight="1">
-      <c r="B84" s="11"/>
+      <c r="B84" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>217</v>
+      </c>
       <c r="AA84" s="6" t="s">
         <v>800</v>
       </c>
@@ -12834,7 +12942,12 @@
       </c>
     </row>
     <row r="89" spans="1:32" ht="24" customHeight="1">
-      <c r="B89" s="11"/>
+      <c r="B89" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>217</v>
+      </c>
       <c r="AA89" s="6" t="s">
         <v>766</v>
       </c>
@@ -12894,6 +13007,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19 B94 B84 B46:B47 B67" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>AA19:AD19</formula1>
@@ -12929,12 +13043,12 @@
       <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="24" customHeight="1">
@@ -12996,7 +13110,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="177.95" customHeight="1">
+    <row r="11" spans="1:3" ht="178" customHeight="1">
       <c r="B11" s="11" t="s">
         <v>818</v>
       </c>
@@ -13387,6 +13501,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B24:B25" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>AA24:AE24</formula1>
@@ -13403,16 +13518,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AH95"/>
   <sheetViews>
-    <sheetView topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.7265625" customWidth="1"/>
+    <col min="2" max="2" width="150.7265625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1796875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="24" customHeight="1">
@@ -13476,7 +13591,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:29" ht="177.95" customHeight="1">
+    <row r="11" spans="1:29" ht="178" customHeight="1">
       <c r="B11" s="11" t="s">
         <v>872</v>
       </c>
@@ -14181,6 +14296,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="16"/>
   <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16 B74 B95" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>AA16:AC16</formula1>

</xml_diff>